<commit_message>
Referências definidas - Inclusão de livro IHC
</commit_message>
<xml_diff>
--- a/CRUZAMENTO DE REFERÊNCIAS.xlsx
+++ b/CRUZAMENTO DE REFERÊNCIAS.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roberto.alves\Documents\PESSOAIS\7º SEMESTRE\TCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Principal\Documents\7º SEMESTRE\TCC\TCC-ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B8B836-51AB-4732-BEE3-272472FDE6F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E40D18-BCE9-4F70-BC57-016ACFBB515C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CB751576-DF97-411A-B7C1-F80F338643F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{CB751576-DF97-411A-B7C1-F80F338643F3}"/>
   </bookViews>
   <sheets>
     <sheet name="IHC" sheetId="3" r:id="rId1"/>
-    <sheet name="assistiva" sheetId="2" r:id="rId2"/>
-    <sheet name="SEO" sheetId="4" r:id="rId3"/>
-    <sheet name="Acessibilidade" sheetId="5" r:id="rId4"/>
+    <sheet name="Planilha1" sheetId="6" r:id="rId2"/>
+    <sheet name="assistiva" sheetId="2" r:id="rId3"/>
+    <sheet name="SEO" sheetId="4" r:id="rId4"/>
+    <sheet name="Acessibilidade" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="282">
   <si>
     <t xml:space="preserve">BARBOSA, Simone D.J., SILVA, Bruno Santana. Interação Humano-Computador. 8º ed. Rio de Janeiro: Elsevier, 2010. </t>
   </si>
@@ -2239,13 +2240,48 @@
   </si>
   <si>
     <t xml:space="preserve">CARTILHA DE ACESSIBILIDADE NA WEB. W3C BRASIL. Disponível em: http://www.w3c.br/pub/Materiais/PublicacoesW3C/cartilha-w3cbr-acessibilidade-webfasciculo-I.pdf. Acesso em: 31 ago. 2015. </t>
+  </si>
+  <si>
+    <t>IHC</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>assistividade / Acessibilidade</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Baranauskas, M. C. C., de Souza, C. S., and Pereira, R. (2012). Grandihc-br: Prospecção de grandes desafios de pesquisa em interação humano-computador no brasil.  In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Com- panion Proceedings of the 11th Brazilian Symposium on Human Factors in Computing Systems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, IHC ’12, pages 63–64, Porto Alegre, Brazil, Brazil. Brazilian Computer So- ciety.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2321,13 +2357,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2342,7 +2398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2385,6 +2441,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2403,7 +2468,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2701,8 +2766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62404FC-054B-4D0D-A8E2-ECCABCA5EA20}">
   <dimension ref="B1:F76"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2727,7 +2792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2738,7 +2803,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
@@ -2749,7 +2814,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="63" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -2760,7 +2825,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2771,7 +2836,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
@@ -2782,7 +2847,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
@@ -2793,7 +2858,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
@@ -2804,7 +2869,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="2:6" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="63" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
@@ -2815,7 +2880,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="63" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -2823,7 +2888,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -2831,327 +2896,327 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D12" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D14" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D15" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D16" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="4:4" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D18" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D19" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D20" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D21" s="8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D25" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D27" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D28" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D29" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D30" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D32" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D33" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D34" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D35" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="4:4" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D36" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D37" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D38" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D39" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D40" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D41" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="4:4" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D42" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="4:4" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D43" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D44" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="4:4" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D45" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="4:4" s="9" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="D46" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D47" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D48" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D49" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D50" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D51" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D52" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D53" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D54" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D55" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="4:4" s="9" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D56" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D57" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D58" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D59" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D60" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D61" s="12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D62" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D63" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D64" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D65" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="4:4" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D66" s="13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D67" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D68" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="4:4" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D69" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D70" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D71" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="4:4" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" ht="63" x14ac:dyDescent="0.25">
       <c r="D72" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D73" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D74" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D75" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="4:4" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D76" s="8" t="s">
         <v>163</v>
       </c>
@@ -3163,10 +3228,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373A79EA-5006-4DA9-8A3B-6782445EC0BE}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" customWidth="1"/>
+    <col min="3" max="3" width="87" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B955EA-6808-4DC5-A186-1E2F288BB352}">
   <dimension ref="B2:I69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -3989,12 +4133,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B59EB2-DFA7-42C0-A869-0556EB1879CF}">
   <dimension ref="B2:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4195,12 +4339,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAFF430-29E2-47B3-B3D7-3B2C822C0337}">
   <dimension ref="B2:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>